<commit_message>
commited the changes of Keyword and TestController
</commit_message>
<xml_diff>
--- a/src/test/java/testData/TestSuite1Data.xlsx
+++ b/src/test/java/testData/TestSuite1Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agraway\Desktop\LifeSpeed-mainy\LifeSpeed-main\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66100A95-8C16-4E52-895E-6C10287032B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65ED42B-6472-4F65-A7DE-C6BAE59345B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7118" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7141" uniqueCount="445">
   <si>
     <t>Gateway_PartnerCode</t>
   </si>
@@ -1305,31 +1305,86 @@
     <t>PrCollected</t>
   </si>
   <si>
-    <t>533598</t>
-  </si>
-  <si>
-    <t>533604</t>
-  </si>
-  <si>
-    <t>533609</t>
-  </si>
-  <si>
-    <t>533649</t>
-  </si>
-  <si>
-    <t>533658</t>
-  </si>
-  <si>
-    <t>533665</t>
-  </si>
-  <si>
-    <t>533672</t>
-  </si>
-  <si>
-    <t>533679</t>
-  </si>
-  <si>
-    <t>533681</t>
+    <t>You have been successfully logged out.
+Please close this browser window.</t>
+  </si>
+  <si>
+    <t>TheCloseText</t>
+  </si>
+  <si>
+    <t>RoleChange</t>
+  </si>
+  <si>
+    <t>534012</t>
+  </si>
+  <si>
+    <t>RoleChangeSU</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>534013</t>
+  </si>
+  <si>
+    <t>534019</t>
+  </si>
+  <si>
+    <t>534039</t>
+  </si>
+  <si>
+    <t>534043</t>
+  </si>
+  <si>
+    <t>534044</t>
+  </si>
+  <si>
+    <t>534047</t>
+  </si>
+  <si>
+    <t>534048</t>
+  </si>
+  <si>
+    <t>534049</t>
+  </si>
+  <si>
+    <t>534050</t>
+  </si>
+  <si>
+    <t>534051</t>
+  </si>
+  <si>
+    <t>534053</t>
+  </si>
+  <si>
+    <t>534054</t>
+  </si>
+  <si>
+    <t>534058</t>
+  </si>
+  <si>
+    <t>534061</t>
+  </si>
+  <si>
+    <t>534064</t>
+  </si>
+  <si>
+    <t>534068</t>
+  </si>
+  <si>
+    <t>534073</t>
+  </si>
+  <si>
+    <t>534074</t>
+  </si>
+  <si>
+    <t>534078</t>
+  </si>
+  <si>
+    <t>534082</t>
+  </si>
+  <si>
+    <t>534085</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1628,6 +1683,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5187,10 +5243,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:DG2"/>
+  <dimension ref="A1:DJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BR1" workbookViewId="0">
-      <selection activeCell="CK16" sqref="CK16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5199,20 +5255,21 @@
     <col min="8" max="8" customWidth="true" width="41.140625"/>
     <col min="9" max="9" customWidth="true" width="26.42578125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="17.28515625"/>
-    <col min="90" max="90" customWidth="true" width="17.7109375"/>
-    <col min="94" max="94" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="107" max="107" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="108" max="108" bestFit="true" customWidth="true" width="10.8515625" collapsed="true"/>
-    <col min="109" max="109" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.85546875"/>
+    <col min="12" max="12" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="13" max="15" customWidth="true" width="17.28515625"/>
+    <col min="92" max="92" customWidth="true" width="17.7109375"/>
+    <col min="96" max="96" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="100" max="100" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="104" max="104" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="110" max="110" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="111" max="111" bestFit="true" customWidth="true" width="10.8515625" collapsed="true"/>
+    <col min="112" max="112" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="113" max="113" bestFit="true" customWidth="true" width="9.203125" collapsed="true"/>
+    <col min="114" max="114" bestFit="true" customWidth="true" width="11.6953125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:111" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:114" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -5243,311 +5300,320 @@
       <c r="J1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="70" t="s">
+        <v>422</v>
+      </c>
+      <c r="L1" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="M1" s="68" t="s">
         <v>337</v>
       </c>
-      <c r="M1" s="68" t="s">
+      <c r="N1" s="68" t="s">
+        <v>420</v>
+      </c>
+      <c r="O1" s="68" t="s">
         <v>338</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="U1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="V1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="W1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="Z1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="AA1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="24" t="s">
+      <c r="AB1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AC1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AD1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="24" t="s">
+      <c r="AE1" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="24" t="s">
+      <c r="AF1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="24" t="s">
+      <c r="AG1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="24" t="s">
+      <c r="AH1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="24" t="s">
+      <c r="AI1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="24" t="s">
+      <c r="AJ1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="24" t="s">
+      <c r="AK1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="24" t="s">
+      <c r="AL1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="24" t="s">
+      <c r="AM1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="24" t="s">
+      <c r="AN1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="24" t="s">
+      <c r="AO1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="24" t="s">
+      <c r="AP1" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="24" t="s">
+      <c r="AQ1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="24" t="s">
+      <c r="AR1" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="AQ1" s="24" t="s">
+      <c r="AS1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AR1" s="24" t="s">
+      <c r="AT1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="AS1" s="24" t="s">
+      <c r="AU1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="AT1" s="24" t="s">
+      <c r="AV1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AU1" s="24" t="s">
+      <c r="AW1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AV1" s="24" t="s">
+      <c r="AX1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="24" t="s">
+      <c r="AY1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" s="23" t="s">
+      <c r="AZ1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AY1" s="22" t="s">
+      <c r="BA1" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="AZ1" s="22" t="s">
+      <c r="BB1" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="BA1" s="22" t="s">
+      <c r="BC1" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="BB1" s="22" t="s">
+      <c r="BD1" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="BC1" s="22" t="s">
+      <c r="BE1" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="BD1" s="22" t="s">
+      <c r="BF1" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="BE1" s="22" t="s">
+      <c r="BG1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="BF1" s="22" t="s">
+      <c r="BH1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="BG1" s="22" t="s">
+      <c r="BI1" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="BH1" s="22" t="s">
+      <c r="BJ1" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="BI1" s="22" t="s">
+      <c r="BK1" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="BJ1" s="22" t="s">
+      <c r="BL1" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="BK1" s="22" t="s">
+      <c r="BM1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="BL1" s="22" t="s">
+      <c r="BN1" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="BM1" s="22" t="s">
+      <c r="BO1" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="BN1" s="22" t="s">
+      <c r="BP1" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="BO1" s="22" t="s">
+      <c r="BQ1" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="BP1" s="22" t="s">
+      <c r="BR1" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="BQ1" s="22" t="s">
+      <c r="BS1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="BR1" s="22" t="s">
+      <c r="BT1" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="BS1" s="22" t="s">
+      <c r="BU1" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="BT1" s="22" t="s">
+      <c r="BV1" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="BU1" s="22" t="s">
+      <c r="BW1" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="BV1" s="22" t="s">
+      <c r="BX1" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="BW1" s="22" t="s">
+      <c r="BY1" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="BX1" s="22" t="s">
+      <c r="BZ1" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="BY1" s="22" t="s">
+      <c r="CA1" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="BZ1" s="22" t="s">
+      <c r="CB1" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="CA1" s="22" t="s">
+      <c r="CC1" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="CB1" s="22" t="s">
+      <c r="CD1" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="CC1" s="22" t="s">
+      <c r="CE1" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="CD1" s="22" t="s">
+      <c r="CF1" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="CE1" s="22" t="s">
+      <c r="CG1" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="CF1" s="22" t="s">
+      <c r="CH1" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="CG1" s="23" t="s">
+      <c r="CI1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="CH1" s="23" t="s">
+      <c r="CJ1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="CI1" s="23" t="s">
+      <c r="CK1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="CJ1" s="21" t="s">
+      <c r="CL1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="CK1" s="25" t="s">
+      <c r="CM1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="CL1" s="19" t="s">
+      <c r="CN1" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="CM1" s="19" t="s">
+      <c r="CO1" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="CN1" s="19" t="s">
+      <c r="CP1" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="CO1" s="19" t="s">
+      <c r="CQ1" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="CP1" s="19" t="s">
+      <c r="CR1" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="CQ1" s="19" t="s">
+      <c r="CS1" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="CR1" s="19" t="s">
+      <c r="CT1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="CS1" s="19" t="s">
+      <c r="CU1" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="CT1" s="19" t="s">
+      <c r="CV1" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="CU1" s="19" t="s">
+      <c r="CW1" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="CV1" s="19" t="s">
+      <c r="CX1" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="CW1" s="19" t="s">
+      <c r="CY1" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="CX1" s="19" t="s">
+      <c r="CZ1" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="CY1" s="19" t="s">
+      <c r="DA1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="CZ1" s="22" t="s">
+      <c r="DB1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="DA1" s="26" t="s">
+      <c r="DC1" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="DD1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="DB1" s="26" t="s">
+      <c r="DE1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="DC1" s="27" t="s">
+      <c r="DF1" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="DD1" s="28" t="s">
+      <c r="DG1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="DE1" s="29" t="s">
+      <c r="DH1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="DF1" s="19" t="s">
+      <c r="DI1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="DG1" s="19" t="s">
+      <c r="DJ1" s="19" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:111" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:114" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -5579,317 +5645,326 @@
         <v>180</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L2" s="64" t="s">
+      <c r="M2" s="64" t="s">
         <v>332</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="66" t="s">
+        <v>320</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AC2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AD2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="10" t="s">
+      <c r="AE2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AF2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AE2" s="10" t="s">
+      <c r="AG2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AF2" s="10" t="s">
+      <c r="AH2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AG2" s="10" t="s">
+      <c r="AI2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="10" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AI2" s="10" t="s">
+      <c r="AK2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="10" t="s">
+      <c r="AL2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" s="10" t="s">
+      <c r="AM2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AL2" s="10" t="s">
+      <c r="AN2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" s="10" t="s">
+      <c r="AO2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AN2" s="10" t="s">
+      <c r="AP2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AO2" s="10" t="s">
+      <c r="AQ2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AP2" s="10" t="s">
+      <c r="AR2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AS2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AR2" s="10" t="s">
+      <c r="AT2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AS2" s="10" t="s">
+      <c r="AU2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AT2" s="10" t="s">
+      <c r="AV2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AU2" s="10" t="s">
+      <c r="AW2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AV2" s="11" t="s">
+      <c r="AX2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="AW2" s="7" t="s">
+      <c r="AY2" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BC2" s="17" t="s">
+      <c r="BE2" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="BD2" s="17" t="s">
+      <c r="BF2" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BK2" s="17" t="s">
+      <c r="BM2" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="BL2" s="17" t="s">
+      <c r="BN2" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="BM2" s="17" t="s">
+      <c r="BO2" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="BN2" s="17" t="s">
+      <c r="BP2" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="BO2" s="17" t="s">
+      <c r="BQ2" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="BP2" s="17" t="s">
+      <c r="BR2" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BY2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BX2" s="17" t="s">
+      <c r="BZ2" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="BY2" s="17" t="s">
+      <c r="CA2" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="BZ2" s="17" t="s">
+      <c r="CB2" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="CA2" s="17" t="s">
+      <c r="CC2" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="CD2" s="17" t="s">
+      <c r="CF2" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="CE2" s="17" t="s">
+      <c r="CG2" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="CF2" s="60" t="s">
+      <c r="CH2" s="60" t="s">
         <v>302</v>
       </c>
-      <c r="CG2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="CH2" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="CI2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="CJ2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CK2" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="CL2" s="69" t="s">
+      <c r="CK2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="CM2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="CN2" s="69" t="s">
         <v>146</v>
       </c>
-      <c r="CM2" s="13" t="s">
+      <c r="CO2" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="CN2" s="13" t="s">
+      <c r="CP2" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="CO2" s="13" t="s">
+      <c r="CQ2" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="CP2" s="13" t="s">
+      <c r="CR2" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="CQ2" s="13" t="s">
+      <c r="CS2" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="CR2" s="13" t="s">
+      <c r="CT2" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="CS2" s="13" t="s">
+      <c r="CU2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="CT2" s="13">
+      <c r="CV2" s="13">
         <v>8218828905</v>
       </c>
-      <c r="CU2" s="32" t="s">
+      <c r="CW2" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="CV2" s="13" t="s">
+      <c r="CX2" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="CW2" s="13" t="s">
+      <c r="CY2" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="CX2" s="13">
+      <c r="CZ2" s="13">
         <v>8218828905</v>
       </c>
-      <c r="CY2" s="32" t="s">
+      <c r="DA2" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="CZ2" s="16" t="s">
+      <c r="DB2" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="DA2" s="15" t="s">
+      <c r="DC2" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="DD2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DB2" s="16" t="s">
+      <c r="DE2" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="DC2" s="15" t="s">
+      <c r="DF2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="DD2" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="DE2" s="7" t="s">
+      <c r="DG2" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="DH2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="DF2" s="1" t="s">
+      <c r="DI2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="DG2" t="s" s="0">
+      <c r="DJ2" t="s" s="0">
         <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BD1:BJ1">
+  <conditionalFormatting sqref="BF1:BL1">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="CU2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="CY2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="L2" r:id="rId3" xr:uid="{FFF5DB8F-5356-4B3F-9CA1-EC35C3F474CC}"/>
+    <hyperlink ref="CW2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="DA2" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{FFF5DB8F-5356-4B3F-9CA1-EC35C3F474CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>